<commit_message>
the systemlogs page and systemlogs script is added
its added to systemlogs branch
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
   <si>
     <t>username</t>
   </si>
@@ -135,13 +138,88 @@
   </si>
   <si>
     <t>userone1</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>deprtsales@gmail.com</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>faveo@2223</t>
+  </si>
+  <si>
+    <t>hostname</t>
+  </si>
+  <si>
+    <t>imap.gmail.com</t>
+  </si>
+  <si>
+    <t>port</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>deptsales11@gmail.com</t>
+  </si>
+  <si>
+    <t>faveo@1234</t>
+  </si>
+  <si>
+    <t>prateek4223@gmail.com</t>
+  </si>
+  <si>
+    <t>rjaditya96@gmail.com</t>
+  </si>
+  <si>
+    <t>Adi@tya9696</t>
+  </si>
+  <si>
+    <t>uname</t>
+  </si>
+  <si>
+    <t>rebel332910@gmail.com</t>
+  </si>
+  <si>
+    <t>rebelverma</t>
+  </si>
+  <si>
+    <t>faveo@2345</t>
+  </si>
+  <si>
+    <t>javalirajeev@gmail.com</t>
+  </si>
+  <si>
+    <t>rajeevjavali</t>
+  </si>
+  <si>
+    <t>Rajeev@1965</t>
+  </si>
+  <si>
+    <t>jayashreerjavali@gmail.com</t>
+  </si>
+  <si>
+    <t>jayajab</t>
+  </si>
+  <si>
+    <t>jaya@1973</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +240,13 @@
       <color rgb="FF72AFD2"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -194,6 +279,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -503,7 +598,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,4 +1002,278 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="5">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
+    <hyperlink ref="B15" r:id="rId3"/>
+    <hyperlink ref="B18" r:id="rId4"/>
+    <hyperlink ref="B19" r:id="rId5" display="Adi@tya9696"/>
+    <hyperlink ref="B20" r:id="rId6"/>
+    <hyperlink ref="B22" r:id="rId7"/>
+    <hyperlink ref="B24" r:id="rId8"/>
+    <hyperlink ref="B26" r:id="rId9"/>
+    <hyperlink ref="B27" r:id="rId10" display="rajeev@1965"/>
+    <hyperlink ref="B28" r:id="rId11"/>
+    <hyperlink ref="B30" r:id="rId12"/>
+    <hyperlink ref="B32" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Installation Scripts In Local
Created a page for installation steps in local and script also.
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7006E16E-FDED-4B26-9F8B-10FBF381A6C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="4935" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="installation" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J25"/>
+  <oleSize ref="A1:K13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>username</t>
   </si>
@@ -213,12 +215,72 @@
   </si>
   <si>
     <t>jaya@1973</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>dbname</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>cpwd</t>
+  </si>
+  <si>
+    <t>pk1</t>
+  </si>
+  <si>
+    <t>pk2</t>
+  </si>
+  <si>
+    <t>pk3</t>
+  </si>
+  <si>
+    <t>pk4</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>kvb422@gmail.com</t>
+  </si>
+  <si>
+    <t>MBUA</t>
+  </si>
+  <si>
+    <t>XQDC</t>
+  </si>
+  <si>
+    <t>WCRX</t>
+  </si>
+  <si>
+    <t>EKMZ</t>
+  </si>
+  <si>
+    <t>tzone</t>
+  </si>
+  <si>
+    <t>asia/kolkata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,6 +446,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -419,6 +498,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,16 +690,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -625,21 +721,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -655,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -664,7 +760,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -672,7 +768,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -683,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -691,7 +787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -699,7 +795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -710,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -718,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -726,7 +822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -734,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -742,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -750,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -758,7 +854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -766,7 +862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -774,7 +870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -785,7 +881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -793,7 +889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -801,7 +897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -809,7 +905,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -817,7 +913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -825,7 +921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -833,7 +929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -841,7 +937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -849,7 +945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -857,7 +953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -865,7 +961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -873,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -881,7 +977,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -889,7 +985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -897,7 +993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -905,7 +1001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -913,7 +1009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -921,7 +1017,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -929,7 +1025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -937,7 +1033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -945,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -953,7 +1049,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -961,7 +1057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -969,7 +1065,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -977,7 +1073,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -987,17 +1083,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="G8" r:id="rId4"/>
-    <hyperlink ref="B15" r:id="rId5"/>
-    <hyperlink ref="B21" r:id="rId6"/>
-    <hyperlink ref="B22" r:id="rId7"/>
-    <hyperlink ref="B31" r:id="rId8"/>
-    <hyperlink ref="B33" r:id="rId9"/>
-    <hyperlink ref="B35" r:id="rId10"/>
-    <hyperlink ref="B36" r:id="rId11"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B21" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B22" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B31" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B33" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B35" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B36" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId12"/>
@@ -1005,23 +1101,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -1032,7 +1128,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
@@ -1043,7 +1139,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>44</v>
       </c>
@@ -1052,7 +1148,7 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>46</v>
       </c>
@@ -1061,7 +1157,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -1069,7 +1165,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>42</v>
       </c>
@@ -1085,7 +1181,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
@@ -1093,14 +1189,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1108,7 +1204,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1212,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
@@ -1124,13 +1220,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1138,7 +1234,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -1146,7 +1242,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>44</v>
       </c>
@@ -1154,7 +1250,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1162,7 +1258,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
@@ -1170,7 +1266,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
@@ -1178,7 +1274,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>40</v>
       </c>
@@ -1186,7 +1282,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
@@ -1194,7 +1290,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1298,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>40</v>
       </c>
@@ -1210,7 +1306,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>42</v>
       </c>
@@ -1218,7 +1314,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
@@ -1228,19 +1324,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B13" r:id="rId2"/>
-    <hyperlink ref="B15" r:id="rId3"/>
-    <hyperlink ref="B18" r:id="rId4"/>
-    <hyperlink ref="B19" r:id="rId5" display="Adi@tya9696"/>
-    <hyperlink ref="B20" r:id="rId6"/>
-    <hyperlink ref="B22" r:id="rId7"/>
-    <hyperlink ref="B24" r:id="rId8"/>
-    <hyperlink ref="B26" r:id="rId9"/>
-    <hyperlink ref="B27" r:id="rId10" display="rajeev@1965"/>
-    <hyperlink ref="B28" r:id="rId11"/>
-    <hyperlink ref="B30" r:id="rId12"/>
-    <hyperlink ref="B32" r:id="rId13"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B18" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B19" r:id="rId5" display="Adi@tya9696" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B20" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B22" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B24" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B26" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B27" r:id="rId10" display="rajeev@1965" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B28" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B30" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B32" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -1248,16 +1344,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -1265,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1276,4 +1372,134 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD740F0A-312C-4C53-AA3A-8241FC153FC6}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{06B1DC07-8918-4431-B212-0EE053CA5A1F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Scripts for email module
Adding email create,edit and delete scripts with different scenarios.
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0040DF23-A3CA-4B3F-9D3C-C73FC9B37D22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{06CC39E5-2B65-4098-8F61-C11A4E398337}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19710" windowHeight="5925" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="4860" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="109">
   <si>
     <t>username</t>
   </si>
@@ -279,13 +279,82 @@
   </si>
   <si>
     <t>un</t>
+  </si>
+  <si>
+    <t>ename</t>
+  </si>
+  <si>
+    <t>epwd</t>
+  </si>
+  <si>
+    <t>incHost</t>
+  </si>
+  <si>
+    <t>outHost</t>
+  </si>
+  <si>
+    <t>faveo64@gmail.com</t>
+  </si>
+  <si>
+    <t>ConfigLink</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>faveo@1122</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>OUTLOOK</t>
+  </si>
+  <si>
+    <t>ONlY INCOM</t>
+  </si>
+  <si>
+    <t>ONLY OUT</t>
+  </si>
+  <si>
+    <t>DEPARTMENT</t>
+  </si>
+  <si>
+    <t>bindu2223@outlook.com</t>
+  </si>
+  <si>
+    <t>Outlook</t>
+  </si>
+  <si>
+    <t>Bheem@2223</t>
+  </si>
+  <si>
+    <t>imap-mail.outlook.com</t>
+  </si>
+  <si>
+    <t>smtp-mail.outlook.com</t>
+  </si>
+  <si>
+    <t>OnlyIncom</t>
+  </si>
+  <si>
+    <t>OnlyOut</t>
+  </si>
+  <si>
+    <t>suprt2223@gmail.com</t>
+  </si>
+  <si>
+    <t>operationdeprtmnt@gmail.com</t>
+  </si>
+  <si>
+    <t>OperationDep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +383,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,6 +433,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1510,31 +1597,166 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664F5BE1-D2BC-4E89-89D6-93D9F6060387}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="12.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:6" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{8BEA6347-EFB6-45DB-8168-CD849A8E1C9B}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{C17E4B3F-6A0D-4950-B0AE-AED84A852D08}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{BBC682C2-7804-42A0-8F99-1D217E2CF76B}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{C01EBBFA-13F3-43B0-B759-77F0BB6C5747}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{71C0AB07-4AF8-4BD5-85F6-8A302B3B9CAA}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{3D6D9C50-CD24-471E-9A17-51D467969C06}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{1DCF4E55-89E5-4BE0-B0FB-8674589C13E7}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{BC6A9CD4-CCE8-4A4F-A945-3FDC10DC15BD}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{7320C402-7E4A-4992-ADFD-27F446BD1C84}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{FF1D114E-9926-4C10-AE01-0666EF452F98}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the code for ddifferent browsers is added
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -4,28 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="loginscript" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="createticket" sheetId="7" r:id="rId6"/>
+    <sheet name="requesterdesc" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>testadmin</t>
-  </si>
-  <si>
     <t>pwd</t>
   </si>
   <si>
@@ -213,6 +212,57 @@
   </si>
   <si>
     <t>jaya@1973</t>
+  </si>
+  <si>
+    <t>agent</t>
+  </si>
+  <si>
+    <t>Agentpass</t>
+  </si>
+  <si>
+    <t>client@gmail.com</t>
+  </si>
+  <si>
+    <t>Client@123</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>robin</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>hood</t>
+  </si>
+  <si>
+    <t>robinhood@gmail.com</t>
+  </si>
+  <si>
+    <t>asdftry</t>
+  </si>
+  <si>
+    <t>qwerhj</t>
+  </si>
+  <si>
+    <t>zxcvbjhkj@gmail.com</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>BossBoss</t>
+  </si>
+  <si>
+    <t>agenta1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is the test </t>
+  </si>
+  <si>
+    <t>this is the test for the agent panel</t>
   </si>
 </sst>
 </file>
@@ -598,7 +648,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,15 +658,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -644,15 +694,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -660,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>123456</v>
@@ -677,18 +727,18 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -696,18 +746,18 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -715,15 +765,15 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -731,15 +781,15 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -747,15 +797,15 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -763,15 +813,15 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -779,18 +829,18 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -798,12 +848,12 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="2">
         <v>12345678</v>
@@ -814,15 +864,15 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -830,15 +880,15 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -846,15 +896,15 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -862,15 +912,15 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -878,15 +928,15 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -894,15 +944,15 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -910,12 +960,12 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" s="2">
         <v>1234567890</v>
@@ -926,15 +976,15 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -942,15 +992,15 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -958,15 +1008,15 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -974,15 +1024,15 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1023,10 +1073,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="5"/>
@@ -1034,10 +1084,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1045,25 +1095,25 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5">
         <v>993</v>
@@ -1071,26 +1121,26 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1102,26 +1152,26 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1132,98 +1182,98 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1249,28 +1299,192 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>55</v>
+      <c r="A1">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the code for creating the ticket from the agent panel and executing in different browser is done
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="loginscript" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="registeruserclient" sheetId="6" r:id="rId5"/>
     <sheet name="createticket" sheetId="7" r:id="rId6"/>
-    <sheet name="requesterdesc" sheetId="8" r:id="rId7"/>
+    <sheet name="createuser" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
   <si>
     <t>username</t>
   </si>
@@ -229,18 +229,12 @@
     <t>fname</t>
   </si>
   <si>
-    <t>robin</t>
-  </si>
-  <si>
     <t>lname</t>
   </si>
   <si>
     <t>hood</t>
   </si>
   <si>
-    <t>robinhood@gmail.com</t>
-  </si>
-  <si>
     <t>asdftry</t>
   </si>
   <si>
@@ -259,10 +253,22 @@
     <t>agenta1</t>
   </si>
   <si>
-    <t xml:space="preserve">this is the test </t>
-  </si>
-  <si>
-    <t>this is the test for the agent panel</t>
+    <t>aamirkhan@gmail.com</t>
+  </si>
+  <si>
+    <t>ganesh</t>
+  </si>
+  <si>
+    <t>ganeshood@gmail.com</t>
+  </si>
+  <si>
+    <t>chicken</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>chickendinner@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -658,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -666,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1362,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1369,15 +1375,15 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1385,7 +1391,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1393,15 +1399,15 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1409,85 +1415,112 @@
         <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D1" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the pages and scripts for change password and forgot password is commited
</commit_message>
<xml_diff>
--- a/data/New Microsoft Excel Worksheet.xlsx
+++ b/data/New Microsoft Excel Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="7860" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1431,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1482,7 +1482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>